<commit_message>
collected new data because there was no change in dimension on old data
</commit_message>
<xml_diff>
--- a/qasm_analysis_10_trap_transfer.xlsx
+++ b/qasm_analysis_10_trap_transfer.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8225978220396727</v>
+        <v>0.09950268380201061</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8225978220396727</v>
+        <v>0.09950268380201061</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F2" t="n">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G2" t="n">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3">
@@ -502,10 +502,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9196473726347113</v>
+        <v>0.5424796504655186</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9196473726347113</v>
+        <v>0.5424796504655186</v>
       </c>
       <c r="D3" t="n">
         <v>25</v>
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9500393645866535</v>
+        <v>0.6509361068228677</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9500393645866535</v>
+        <v>0.6509361068228677</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F4" t="n">
         <v>50</v>
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7187462112981424</v>
+        <v>0.004638037914405086</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7187462112981424</v>
+        <v>0.00408726988385714</v>
       </c>
       <c r="D5" t="n">
-        <v>191</v>
+        <v>245</v>
       </c>
       <c r="E5" t="n">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="F5" t="n">
         <v>271</v>
@@ -577,10 +577,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9888910438521609</v>
+        <v>0.9391719980261437</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9888910438521609</v>
+        <v>0.9391719980261437</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3178754915054511</v>
+        <v>5.411969235495265e-05</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3178754915054511</v>
+        <v>3.938179468674988e-05</v>
       </c>
       <c r="D7" t="n">
-        <v>800</v>
+        <v>851</v>
       </c>
       <c r="E7" t="n">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="F7" t="n">
         <v>898</v>
@@ -627,16 +627,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8104600979121517</v>
+        <v>0.08946727459308944</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8104600979121517</v>
+        <v>0.08588199538181801</v>
       </c>
       <c r="D8" t="n">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="E8" t="n">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F8" t="n">
         <v>172</v>
@@ -652,13 +652,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6770278940676773</v>
+        <v>0.03507900269087775</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6770278940676773</v>
+        <v>0.03430511105638601</v>
       </c>
       <c r="D9" t="n">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E9" t="n">
         <v>271</v>
@@ -677,16 +677,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8692576402050464</v>
+        <v>0.3857449803705244</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8692576402050464</v>
+        <v>0.381939279255351</v>
       </c>
       <c r="D10" t="n">
         <v>39</v>
       </c>
       <c r="E10" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="n">
         <v>128</v>
@@ -702,22 +702,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1626527688677107</v>
+        <v>2.169669594463701e-09</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1626527688677107</v>
+        <v>1.192174361104931e-09</v>
       </c>
       <c r="D11" t="n">
-        <v>1074</v>
+        <v>1173</v>
       </c>
       <c r="E11" t="n">
-        <v>1074</v>
+        <v>1112</v>
       </c>
       <c r="F11" t="n">
-        <v>1483</v>
+        <v>1486</v>
       </c>
       <c r="G11" t="n">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="12">
@@ -727,16 +727,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7200033059411529</v>
+        <v>0.03923822944299557</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7200033059411529</v>
+        <v>0.03923822944299557</v>
       </c>
       <c r="D12" t="n">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="E12" t="n">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="F12" t="n">
         <v>312</v>
@@ -752,16 +752,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8875514296351712</v>
+        <v>0.5035560325870317</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8875514296351712</v>
+        <v>0.5019982358591089</v>
       </c>
       <c r="D13" t="n">
         <v>88</v>
       </c>
       <c r="E13" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F13" t="n">
         <v>92</v>
@@ -777,13 +777,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9571884689245493</v>
+        <v>0.7688953153587761</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9571884689245493</v>
+        <v>0.7617814239549737</v>
       </c>
       <c r="D14" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E14" t="n">
         <v>25</v>
@@ -802,19 +802,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.964076289899667</v>
+        <v>0.7894068617535624</v>
       </c>
       <c r="C15" t="n">
-        <v>0.964076289899667</v>
+        <v>0.7868686898597245</v>
       </c>
       <c r="D15" t="n">
         <v>18</v>
       </c>
       <c r="E15" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F15" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G15" t="n">
         <v>31</v>
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9192232557156448</v>
+        <v>0.6266129947137067</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9192232557156448</v>
+        <v>0.6266129947137067</v>
       </c>
       <c r="D16" t="n">
         <v>62</v>
@@ -852,22 +852,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9349559527393196</v>
+        <v>0.5597822348226835</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9349559527393196</v>
+        <v>0.5597822348226835</v>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F17" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data over 30 runs
</commit_message>
<xml_diff>
--- a/qasm_analysis_10_trap_transfer.xlsx
+++ b/qasm_analysis_10_trap_transfer.xlsx
@@ -480,10 +480,10 @@
         <v>0.09950268380201061</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09950268380201061</v>
+        <v>0.01365594787041438</v>
       </c>
       <c r="D2" t="n">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="E2" t="n">
         <v>38</v>
@@ -492,7 +492,7 @@
         <v>192</v>
       </c>
       <c r="G2" t="n">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.004638037914405086</v>
+        <v>0.006067347585136266</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00408726988385714</v>
+        <v>0.003836920719329858</v>
       </c>
       <c r="D5" t="n">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E5" t="n">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="F5" t="n">
         <v>271</v>
       </c>
       <c r="G5" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.411969235495265e-05</v>
+        <v>5.722375326022583e-05</v>
       </c>
       <c r="C7" t="n">
-        <v>3.938179468674988e-05</v>
+        <v>3.851297747070992e-05</v>
       </c>
       <c r="D7" t="n">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="E7" t="n">
-        <v>794</v>
+        <v>784</v>
       </c>
       <c r="F7" t="n">
         <v>898</v>
@@ -627,16 +627,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08946727459308944</v>
+        <v>0.09225411966263156</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08588199538181801</v>
+        <v>0.08077165916344395</v>
       </c>
       <c r="D8" t="n">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E8" t="n">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F8" t="n">
         <v>172</v>
@@ -652,16 +652,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03507900269087775</v>
+        <v>0.0383531350879566</v>
       </c>
       <c r="C9" t="n">
-        <v>0.03430511105638601</v>
+        <v>0.03226381414977151</v>
       </c>
       <c r="D9" t="n">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="E9" t="n">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="F9" t="n">
         <v>306</v>
@@ -677,22 +677,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3857449803705244</v>
+        <v>0.3970927852420561</v>
       </c>
       <c r="C10" t="n">
-        <v>0.381939279255351</v>
+        <v>0.3763010113054139</v>
       </c>
       <c r="D10" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E10" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" t="n">
         <v>128</v>
       </c>
       <c r="G10" t="n">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
@@ -702,22 +702,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.169669594463701e-09</v>
+        <v>2.477806270654973e-09</v>
       </c>
       <c r="C11" t="n">
-        <v>1.192174361104931e-09</v>
+        <v>1.101265678433875e-09</v>
       </c>
       <c r="D11" t="n">
-        <v>1173</v>
+        <v>1181</v>
       </c>
       <c r="E11" t="n">
-        <v>1112</v>
+        <v>1098</v>
       </c>
       <c r="F11" t="n">
-        <v>1486</v>
+        <v>1488</v>
       </c>
       <c r="G11" t="n">
-        <v>1484</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="12">
@@ -752,16 +752,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5035560325870317</v>
+        <v>0.507471706605126</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5019982358591089</v>
+        <v>0.5004452583181059</v>
       </c>
       <c r="D13" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E13" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F13" t="n">
         <v>92</v>
@@ -780,10 +780,10 @@
         <v>0.7688953153587761</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7617814239549737</v>
+        <v>0.7589543307708074</v>
       </c>
       <c r="D14" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" t="n">
         <v>25</v>
@@ -830,10 +830,10 @@
         <v>0.6266129947137067</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6266129947137067</v>
+        <v>0.6250617265957956</v>
       </c>
       <c r="D16" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E16" t="n">
         <v>62</v>

</xml_diff>